<commit_message>
11-01-2018 work done mostly on python
</commit_message>
<xml_diff>
--- a/worklog/work log.xlsx
+++ b/worklog/work log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -60,7 +60,13 @@
     <t>vi editor commands</t>
   </si>
   <si>
-    <t>python basics</t>
+    <t>python basics(overview,basic syntax,variables,operators,decision making,loops</t>
+  </si>
+  <si>
+    <t>python basics( number string list tuple dictionary d&amp;t</t>
+  </si>
+  <si>
+    <t>python: functions modules file I/O exceptions,OOP reg</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -387,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43109</v>
       </c>
@@ -653,16 +659,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43110</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43111</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>

</xml_diff>

<commit_message>
django clinical trials search app
</commit_message>
<xml_diff>
--- a/worklog/work log.xlsx
+++ b/worklog/work log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>flight booking app ui</t>
+  </si>
+  <si>
+    <t>clinical trial search app</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,6 +832,22 @@
         <v>26</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>